<commit_message>
updates shotClock, gameOver, and swishCollision functions properly
</commit_message>
<xml_diff>
--- a/project-module-1-schedule.xlsx
+++ b/project-module-1-schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamfiallos/Desktop/ironhack/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamfiallos/Desktop/ironhack/project-module-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C18C364-04CA-0F48-841C-9862173D693A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34255D6F-E3E2-C046-8698-800E1ABC42D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16660" xr2:uid="{C6BF5BB3-CB48-A846-AB03-40586D742505}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="19460" windowHeight="14420" xr2:uid="{C6BF5BB3-CB48-A846-AB03-40586D742505}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Hoops</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>MODULE 1 PROJECT</t>
+  </si>
+  <si>
+    <t>Game Over</t>
   </si>
 </sst>
 </file>
@@ -494,25 +497,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -520,9 +508,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -546,6 +531,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -865,7 +868,7 @@
   <dimension ref="B3:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,34 +886,34 @@
   <sheetData>
     <row r="3" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="30"/>
     </row>
     <row r="5" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="18"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -919,25 +922,25 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -946,112 +949,114 @@
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="20"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="20"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="20"/>
+      <c r="H9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="20"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="20"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>